<commit_message>
B1.03 - model update
</commit_message>
<xml_diff>
--- a/Log/em_log.xlsx
+++ b/Log/em_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\UKMOD\WORKING\Log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\UKMOD\MODELS\PRIVATE\Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15050BC1-2B73-43FC-A282-AAB3C5EF2843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4643D7F4-BF53-47C3-8103-1D3B3CA96696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="27330" windowHeight="14925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="em_log" sheetId="17593" r:id="rId1"/>
@@ -20,8 +20,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="1420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="1433">
   <si>
     <t>Date</t>
   </si>
@@ -5386,7 +5390,7 @@
     <t>Adjusted settings files to organise extensions in run window in alphabetical order</t>
   </si>
   <si>
-    <t>UK16</t>
+    <t>UK16.XML</t>
   </si>
   <si>
     <t>2022-26</t>
@@ -5396,6 +5400,57 @@
   </si>
   <si>
     <t>Added support for triple lock</t>
+  </si>
+  <si>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <t xml:space="preserve">Merged with version A3.26 and saved as </t>
+    </r>
+    <r xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>B1.02</t>
+    </r>
+  </si>
+  <si>
+    <t>B1.02</t>
+  </si>
+  <si>
+    <t>2016-19</t>
+  </si>
+  <si>
+    <t>2010-2015</t>
+  </si>
+  <si>
+    <t>LDN</t>
+  </si>
+  <si>
+    <t>added switch that allows for keeping households from London only</t>
+  </si>
+  <si>
+    <t>uk16.XML</t>
+  </si>
+  <si>
+    <t>2023-26</t>
+  </si>
+  <si>
+    <t>ITThresh1/4_S, ITRate1/5_S, SCWHA, BScStG*, BScBSF0, BScBSF1to2, CASup</t>
+  </si>
+  <si>
+    <t>Parameter adjustments to reflect Scottish Budget</t>
+  </si>
+  <si>
+    <t>2019-26</t>
+  </si>
+  <si>
+    <t>BScBSF0 and BScBSF1to2</t>
+  </si>
+  <si>
+    <t>Parameters assigned wrong way around</t>
   </si>
 </sst>
 </file>
@@ -6279,10 +6334,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:I760"/>
+  <dimension ref="A1:I769"/>
   <sheetViews>
     <sheetView tabSelected="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A895" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A915" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -24493,6 +24548,232 @@
         <v>1419</v>
       </c>
     </row>
+    <row r="761">
+      <c r="A761" s="61">
+        <v>44902</v>
+      </c>
+      <c r="B761" s="53" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C761" s="53" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D761" s="53" t="s">
+        <v>1420</v>
+      </c>
+      <c r="E761" s="53"/>
+      <c r="F761" s="53"/>
+      <c r="G761" s="53"/>
+      <c r="H761" s="53"/>
+    </row>
+    <row r="762">
+      <c r="A762" s="47">
+        <v>44907</v>
+      </c>
+      <c r="B762" s="46" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C762" s="46" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D762" s="46" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E762" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="F762" s="46" t="s">
+        <v>1422</v>
+      </c>
+      <c r="G762" s="46" t="s">
+        <v>1355</v>
+      </c>
+      <c r="H762" s="46" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" s="47">
+        <v>44907</v>
+      </c>
+      <c r="B763" s="46" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C763" s="46" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D763" s="46" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E763" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="F763" s="46" t="s">
+        <v>1423</v>
+      </c>
+      <c r="G763" s="46" t="s">
+        <v>1355</v>
+      </c>
+      <c r="H763" s="46" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" s="47">
+        <v>44907</v>
+      </c>
+      <c r="B764" s="46" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C764" s="46" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D764" s="46" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E764" s="46" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F764" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G764" s="46" t="s">
+        <v>1424</v>
+      </c>
+      <c r="H764" s="46" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" s="47">
+        <v>44907</v>
+      </c>
+      <c r="B765" s="46" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C765" s="46" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D765" s="46" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E765" s="46" t="s">
+        <v>786</v>
+      </c>
+      <c r="F765" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G765" s="48">
+        <v>12.5</v>
+      </c>
+      <c r="H765" s="46" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" s="47">
+        <v>44907</v>
+      </c>
+      <c r="B766" s="46" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C766" s="46" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D766" s="46" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E766" s="46" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F766" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G766" s="46" t="s">
+        <v>1424</v>
+      </c>
+      <c r="H766" s="46" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" s="47">
+        <v>44907</v>
+      </c>
+      <c r="B767" s="46" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C767" s="46" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D767" s="46" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E767" s="46" t="s">
+        <v>786</v>
+      </c>
+      <c r="F767" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G767" s="48">
+        <v>12.5</v>
+      </c>
+      <c r="H767" s="46" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" s="47">
+        <v>44911</v>
+      </c>
+      <c r="B768" s="44" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C768" s="46" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D768" s="46" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E768" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="F768" s="46" t="s">
+        <v>1427</v>
+      </c>
+      <c r="G768" s="46" t="s">
+        <v>1428</v>
+      </c>
+      <c r="H768" s="46" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" s="47">
+        <v>44911</v>
+      </c>
+      <c r="B769" s="44" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C769" s="46" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D769" s="46" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E769" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="F769" s="46" t="s">
+        <v>1430</v>
+      </c>
+      <c r="G769" s="44" t="s">
+        <v>1431</v>
+      </c>
+      <c r="H769" s="44" t="s">
+        <v>1432</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="70" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>